<commit_message>
Add midway noise monitor info
</commit_message>
<xml_diff>
--- a/Data/warehouse_athena_map.xlsx
+++ b/Data/warehouse_athena_map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Scratch Space\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wridgew\Documents\wiki_content\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_930C1B14328F8466F8F101C9E835FF6ADE7DA7F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34BFD787-AAE3-4C47-8888-A86BB03E0356}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B3539E-7706-45F6-A2F5-AB7253723A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$180</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$181</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="384">
   <si>
     <t>Top-level Warehouse Folder</t>
   </si>
@@ -1180,13 +1180,22 @@
   </si>
   <si>
     <t>RPIE mailers containing address, PINs, and RPIE codes.</t>
+  </si>
+  <si>
+    <t>environment/midway_noise_monitor/</t>
+  </si>
+  <si>
+    <t>spatial.midway_noise_monitor</t>
+  </si>
+  <si>
+    <t>Midway noise monitor locations and readings.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1222,6 +1231,11 @@
       <sz val="10"/>
       <name val="JetBrains Mono"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="JetBrains Mono"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1250,7 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1284,7 +1298,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -1294,9 +1314,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1580,27 +1597,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I180"/>
+  <dimension ref="A1:I181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="D2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.625" customWidth="1"/>
-    <col min="4" max="4" width="34.375" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
     <col min="7" max="7" width="47" customWidth="1"/>
-    <col min="8" max="8" width="113.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="113.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1656,7 +1673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1683,7 +1700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1710,7 +1727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1737,7 +1754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1764,7 +1781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1791,7 +1808,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1814,11 +1831,11 @@
       <c r="G8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1841,9 +1858,9 @@
       <c r="G9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1866,9 +1883,9 @@
       <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1891,9 +1908,9 @@
       <c r="G11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1916,9 +1933,9 @@
       <c r="G12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1941,9 +1958,9 @@
       <c r="G13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1966,9 +1983,9 @@
       <c r="G14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1991,9 +2008,9 @@
       <c r="G15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -2016,9 +2033,9 @@
       <c r="G16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -2041,9 +2058,9 @@
       <c r="G17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -2066,9 +2083,9 @@
       <c r="G18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -2091,9 +2108,9 @@
       <c r="G19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -2116,9 +2133,9 @@
       <c r="G20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -2141,9 +2158,9 @@
       <c r="G21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -2166,9 +2183,9 @@
       <c r="G22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
@@ -2191,9 +2208,9 @@
       <c r="G23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -2216,9 +2233,9 @@
       <c r="G24" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2241,11 +2258,11 @@
       <c r="G25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -2268,9 +2285,9 @@
       <c r="G26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -2293,9 +2310,9 @@
       <c r="G27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="H27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -2318,11 +2335,11 @@
       <c r="G28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -2345,9 +2362,9 @@
       <c r="G29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
@@ -2370,9 +2387,9 @@
       <c r="G30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2395,9 +2412,9 @@
       <c r="G31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="H31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -2424,7 +2441,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -2451,7 +2468,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="9" customFormat="1">
+    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>72</v>
       </c>
@@ -2468,9 +2485,9 @@
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="18"/>
-    </row>
-    <row r="35" spans="1:8" s="9" customFormat="1">
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>72</v>
       </c>
@@ -2487,9 +2504,9 @@
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -2516,7 +2533,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
@@ -2539,11 +2556,11 @@
       <c r="G37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="18" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>79</v>
       </c>
@@ -2566,9 +2583,9 @@
       <c r="G38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="15"/>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="H38" s="16"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
@@ -2591,9 +2608,9 @@
       <c r="G39" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H39" s="15"/>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>79</v>
       </c>
@@ -2616,9 +2633,9 @@
       <c r="G40" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H40" s="15"/>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>79</v>
       </c>
@@ -2641,9 +2658,9 @@
       <c r="G41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H41" s="15"/>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
@@ -2666,9 +2683,9 @@
       <c r="G42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="15"/>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>79</v>
       </c>
@@ -2691,9 +2708,9 @@
       <c r="G43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H43" s="15"/>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="H43" s="16"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>79</v>
       </c>
@@ -2716,9 +2733,9 @@
       <c r="G44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H44" s="15"/>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="H44" s="16"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
@@ -2741,9 +2758,9 @@
       <c r="G45" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H45" s="15"/>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="H45" s="16"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
@@ -2766,9 +2783,9 @@
       <c r="G46" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="15"/>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>79</v>
       </c>
@@ -2791,9 +2808,9 @@
       <c r="G47" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="15"/>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>79</v>
       </c>
@@ -2816,9 +2833,9 @@
       <c r="G48" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H48" s="15"/>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>79</v>
       </c>
@@ -2841,9 +2858,9 @@
       <c r="G49" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="15"/>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>79</v>
       </c>
@@ -2866,9 +2883,9 @@
       <c r="G50" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H50" s="15"/>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="H50" s="16"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
@@ -2891,9 +2908,9 @@
       <c r="G51" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="15"/>
-    </row>
-    <row r="52" spans="1:8">
+      <c r="H51" s="16"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
@@ -2916,9 +2933,9 @@
       <c r="G52" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H52" s="15"/>
-    </row>
-    <row r="53" spans="1:8">
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>79</v>
       </c>
@@ -2941,9 +2958,9 @@
       <c r="G53" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H53" s="15"/>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="H53" s="16"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>79</v>
       </c>
@@ -2966,9 +2983,9 @@
       <c r="G54" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H54" s="15"/>
-    </row>
-    <row r="55" spans="1:8">
+      <c r="H54" s="16"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -2991,9 +3008,9 @@
       <c r="G55" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H55" s="15"/>
-    </row>
-    <row r="56" spans="1:8">
+      <c r="H55" s="16"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
@@ -3016,9 +3033,9 @@
       <c r="G56" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H56" s="15"/>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="H56" s="16"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>79</v>
       </c>
@@ -3041,9 +3058,9 @@
       <c r="G57" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H57" s="15"/>
-    </row>
-    <row r="58" spans="1:8">
+      <c r="H57" s="16"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>79</v>
       </c>
@@ -3066,9 +3083,9 @@
       <c r="G58" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H58" s="15"/>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="H58" s="16"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>79</v>
       </c>
@@ -3091,9 +3108,9 @@
       <c r="G59" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H59" s="15"/>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="H59" s="16"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>79</v>
       </c>
@@ -3116,9 +3133,9 @@
       <c r="G60" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H60" s="15"/>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="H60" s="16"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>79</v>
       </c>
@@ -3141,9 +3158,9 @@
       <c r="G61" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H61" s="15"/>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="H61" s="16"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
@@ -3166,9 +3183,9 @@
       <c r="G62" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H62" s="15"/>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="H62" s="16"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>79</v>
       </c>
@@ -3191,9 +3208,9 @@
       <c r="G63" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H63" s="15"/>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>79</v>
       </c>
@@ -3216,9 +3233,9 @@
       <c r="G64" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H64" s="15"/>
-    </row>
-    <row r="65" spans="1:9">
+      <c r="H64" s="16"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>79</v>
       </c>
@@ -3241,9 +3258,9 @@
       <c r="G65" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H65" s="15"/>
-    </row>
-    <row r="66" spans="1:9">
+      <c r="H65" s="16"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>79</v>
       </c>
@@ -3266,9 +3283,9 @@
       <c r="G66" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H66" s="15"/>
-    </row>
-    <row r="67" spans="1:9">
+      <c r="H66" s="16"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>79</v>
       </c>
@@ -3291,9 +3308,9 @@
       <c r="G67" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H67" s="15"/>
-    </row>
-    <row r="68" spans="1:9">
+      <c r="H67" s="16"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>144</v>
       </c>
@@ -3320,7 +3337,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
@@ -3347,7 +3364,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>149</v>
       </c>
@@ -3374,7 +3391,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>149</v>
       </c>
@@ -3401,7 +3418,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>160</v>
       </c>
@@ -3428,7 +3445,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="11" customFormat="1" ht="14.25">
+    <row r="73" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>164</v>
       </c>
@@ -3458,7 +3475,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="11" customFormat="1" ht="14.25">
+    <row r="74" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>164</v>
       </c>
@@ -3488,7 +3505,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="11" customFormat="1" ht="14.25">
+    <row r="75" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>164</v>
       </c>
@@ -3518,7 +3535,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>164</v>
       </c>
@@ -3545,7 +3562,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>164</v>
       </c>
@@ -3572,7 +3589,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>164</v>
       </c>
@@ -3599,7 +3616,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>164</v>
       </c>
@@ -3622,11 +3639,11 @@
       <c r="G79" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H79" s="19" t="s">
+      <c r="H79" s="17" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>164</v>
       </c>
@@ -3649,9 +3666,9 @@
       <c r="G80" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H80" s="19"/>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="H80" s="17"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>164</v>
       </c>
@@ -3674,9 +3691,9 @@
       <c r="G81" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H81" s="19"/>
-    </row>
-    <row r="82" spans="1:9" s="11" customFormat="1" ht="14.25">
+      <c r="H81" s="17"/>
+    </row>
+    <row r="82" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>164</v>
       </c>
@@ -3706,7 +3723,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>164</v>
       </c>
@@ -3729,11 +3746,11 @@
       <c r="G83" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H83" s="15" t="s">
+      <c r="H83" s="16" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>164</v>
       </c>
@@ -3756,9 +3773,9 @@
       <c r="G84" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H84" s="15"/>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="H84" s="16"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>164</v>
       </c>
@@ -3781,11 +3798,11 @@
       <c r="G85" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H85" s="15" t="s">
+      <c r="H85" s="16" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>164</v>
       </c>
@@ -3808,9 +3825,9 @@
       <c r="G86" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H86" s="15"/>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="H86" s="16"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>164</v>
       </c>
@@ -3833,9 +3850,9 @@
       <c r="G87" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H87" s="15"/>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="H87" s="16"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>164</v>
       </c>
@@ -3858,9 +3875,9 @@
       <c r="G88" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H88" s="15"/>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="H88" s="16"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>164</v>
       </c>
@@ -3883,9 +3900,9 @@
       <c r="G89" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H89" s="15"/>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="H89" s="16"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>164</v>
       </c>
@@ -3908,9 +3925,9 @@
       <c r="G90" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H90" s="15"/>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="H90" s="16"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>164</v>
       </c>
@@ -3933,9 +3950,9 @@
       <c r="G91" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H91" s="15"/>
-    </row>
-    <row r="92" spans="1:9">
+      <c r="H91" s="16"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>164</v>
       </c>
@@ -3958,9 +3975,9 @@
       <c r="G92" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H92" s="15"/>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="H92" s="16"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>164</v>
       </c>
@@ -3983,9 +4000,9 @@
       <c r="G93" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H93" s="15"/>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="H93" s="16"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>164</v>
       </c>
@@ -4008,9 +4025,9 @@
       <c r="G94" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H94" s="15"/>
-    </row>
-    <row r="95" spans="1:9">
+      <c r="H94" s="16"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>164</v>
       </c>
@@ -4033,9 +4050,9 @@
       <c r="G95" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H95" s="15"/>
-    </row>
-    <row r="96" spans="1:9">
+      <c r="H95" s="16"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>164</v>
       </c>
@@ -4058,9 +4075,9 @@
       <c r="G96" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H96" s="15"/>
-    </row>
-    <row r="97" spans="1:9">
+      <c r="H96" s="16"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>164</v>
       </c>
@@ -4083,9 +4100,9 @@
       <c r="G97" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H97" s="15"/>
-    </row>
-    <row r="98" spans="1:9">
+      <c r="H97" s="16"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>164</v>
       </c>
@@ -4108,9 +4125,9 @@
       <c r="G98" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H98" s="15"/>
-    </row>
-    <row r="99" spans="1:9" s="11" customFormat="1" ht="14.25">
+      <c r="H98" s="16"/>
+    </row>
+    <row r="99" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>164</v>
       </c>
@@ -4140,7 +4157,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="11" customFormat="1" ht="14.25">
+    <row r="100" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>164</v>
       </c>
@@ -4170,7 +4187,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>164</v>
       </c>
@@ -4193,11 +4210,11 @@
       <c r="G101" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H101" s="15" t="s">
+      <c r="H101" s="16" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>164</v>
       </c>
@@ -4220,9 +4237,9 @@
       <c r="G102" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H102" s="15"/>
-    </row>
-    <row r="103" spans="1:9">
+      <c r="H102" s="16"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>164</v>
       </c>
@@ -4249,7 +4266,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>164</v>
       </c>
@@ -4276,7 +4293,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>164</v>
       </c>
@@ -4303,7 +4320,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="11" customFormat="1" ht="14.25">
+    <row r="106" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>164</v>
       </c>
@@ -4333,7 +4350,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>164</v>
       </c>
@@ -4360,7 +4377,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>164</v>
       </c>
@@ -4387,214 +4404,214 @@
         <v>243</v>
       </c>
     </row>
-    <row r="109" spans="1:9" s="11" customFormat="1" ht="14.25">
+    <row r="109" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>164</v>
       </c>
       <c r="B109" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C109" s="10" t="str">
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-environment-midway_noise.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-environment-midway_noise.R")</f>
+        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-environment-midway_noise.R</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H109" s="15" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C109" s="10" t="str">
+      <c r="C110" s="10" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-environment.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-environment.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-environment.R</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D110" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E109" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F109" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G109" s="4" t="s">
+      <c r="E110" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G110" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H109" s="13" t="s">
+      <c r="H110" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="I109" s="11" t="s">
+      <c r="I110" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
-      <c r="A110" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B110" s="1" t="s">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C110" s="2" t="str">
+      <c r="C111" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-other.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-other.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-other.R</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G110" s="1" t="s">
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H110" s="12" t="s">
+      <c r="H111" s="12" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="111" spans="1:9" s="11" customFormat="1" ht="14.25">
-      <c r="A111" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B111" s="4" t="s">
+    <row r="112" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C111" s="10" t="str">
+      <c r="C112" s="10" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-other.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-other.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-other.R</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D112" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E111" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G111" s="4" t="s">
+      <c r="E112" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G112" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="H111" s="13" t="s">
+      <c r="H112" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="I111" s="11" t="s">
+      <c r="I112" s="11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
-      <c r="A112" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B112" s="1" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C112" s="2" t="str">
+      <c r="C113" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-other.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-other.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-other.R</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G112" s="1" t="s">
+      <c r="E113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H112" s="12" t="s">
+      <c r="H113" s="12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
-      <c r="A113" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B113" s="1" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C113" s="2" t="str">
+      <c r="C114" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-parcel.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-parcel.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-parcel.R</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G113" s="1" t="s">
+      <c r="E114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G114" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H113" s="12" t="s">
+      <c r="H114" s="12" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
-      <c r="A114" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B114" s="1" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C114" s="2" t="str">
+      <c r="C115" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-police.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-police.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-police.R</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G114" s="1" t="s">
+      <c r="E115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H114" s="12" t="s">
+      <c r="H115" s="12" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
-      <c r="A115" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B115" s="1" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B116" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C115" s="2" t="str">
-        <f t="shared" ref="C115:C122" si="4">HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-political.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R")</f>
+      <c r="C116" s="2" t="str">
+        <f t="shared" ref="C116:C123" si="4">HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-political.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H115" s="12" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8">
-      <c r="A116" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C116" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>12</v>
@@ -4605,23 +4622,23 @@
       <c r="G116" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H116" s="14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="H116" s="12" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C117" s="2" t="str">
         <f t="shared" si="4"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>12</v>
@@ -4632,23 +4649,23 @@
       <c r="G117" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H117" s="5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="H117" s="14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C118" s="2" t="str">
         <f t="shared" si="4"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>12</v>
@@ -4659,23 +4676,23 @@
       <c r="G118" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H118" s="12" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="H118" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C119" s="2" t="str">
         <f t="shared" si="4"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>12</v>
@@ -4687,22 +4704,22 @@
         <v>167</v>
       </c>
       <c r="H119" s="12" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C120" s="2" t="str">
         <f t="shared" si="4"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>12</v>
@@ -4713,23 +4730,23 @@
       <c r="G120" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H120" s="14" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="H120" s="12" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C121" s="2" t="str">
         <f t="shared" si="4"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>12</v>
@@ -4741,22 +4758,22 @@
         <v>167</v>
       </c>
       <c r="H121" s="14" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C122" s="2" t="str">
         <f t="shared" si="4"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>12</v>
@@ -4768,22 +4785,22 @@
         <v>167</v>
       </c>
       <c r="H122" s="14" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C123" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-school.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R")</f>
-        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R</v>
+        <f t="shared" si="4"/>
+        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-political.R</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>12</v>
@@ -4794,16 +4811,16 @@
       <c r="G123" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H123" s="15" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="H123" s="14" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C124" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-school.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R")</f>
@@ -4821,14 +4838,16 @@
       <c r="G124" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H124" s="15"/>
-    </row>
-    <row r="125" spans="1:8">
+      <c r="H124" s="16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C125" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-school.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R")</f>
@@ -4846,21 +4865,21 @@
       <c r="G125" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H125" s="15"/>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="H125" s="16"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C126" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-school.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>12</v>
@@ -4871,23 +4890,21 @@
       <c r="G126" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H126" s="12" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8">
+      <c r="H126" s="16"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C127" s="2" t="str">
-        <f t="shared" ref="C127:C133" si="5">HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R")</f>
-        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-school.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R")</f>
+        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-school.R</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>12</v>
@@ -4898,23 +4915,23 @@
       <c r="G127" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H127" s="15" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="H127" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C128" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C128:C134" si="5">HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>12</v>
@@ -4925,21 +4942,23 @@
       <c r="G128" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H128" s="15"/>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="H128" s="16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C129" s="2" t="str">
         <f t="shared" si="5"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>12</v>
@@ -4950,21 +4969,21 @@
       <c r="G129" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H129" s="15"/>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="H129" s="16"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C130" s="2" t="str">
         <f t="shared" si="5"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>12</v>
@@ -4975,21 +4994,21 @@
       <c r="G130" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H130" s="15"/>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="H130" s="16"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C131" s="2" t="str">
         <f t="shared" si="5"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>12</v>
@@ -5000,21 +5019,21 @@
       <c r="G131" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H131" s="15"/>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="H131" s="16"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C132" s="2" t="str">
         <f t="shared" si="5"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>12</v>
@@ -5025,21 +5044,21 @@
       <c r="G132" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H132" s="15"/>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="H132" s="16"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C133" s="2" t="str">
         <f t="shared" si="5"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>12</v>
@@ -5050,21 +5069,21 @@
       <c r="G133" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H133" s="15"/>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="H133" s="16"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C134" s="2" t="str">
-        <f t="shared" ref="C134:C140" si="6">HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R")</f>
-        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R</v>
+        <f t="shared" si="5"/>
+        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-tax.R</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>12</v>
@@ -5075,23 +5094,21 @@
       <c r="G134" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H134" s="14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="H134" s="16"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C135" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="C135:C141" si="6">HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>12</v>
@@ -5102,16 +5119,16 @@
       <c r="G135" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H135" s="17" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="H135" s="14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C136" s="2" t="str">
         <f t="shared" si="6"/>
@@ -5129,14 +5146,16 @@
       <c r="G136" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H136" s="17"/>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="H136" s="19" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C137" s="2" t="str">
         <f t="shared" si="6"/>
@@ -5154,21 +5173,21 @@
       <c r="G137" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H137" s="17"/>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="H137" s="19"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C138" s="2" t="str">
         <f t="shared" si="6"/>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>12</v>
@@ -5179,16 +5198,14 @@
       <c r="G138" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H138" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="H138" s="19"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C139" s="2" t="str">
         <f t="shared" si="6"/>
@@ -5206,14 +5223,16 @@
       <c r="G139" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H139" s="15"/>
-    </row>
-    <row r="140" spans="1:8">
+      <c r="H139" s="16" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C140" s="2" t="str">
         <f t="shared" si="6"/>
@@ -5231,65 +5250,69 @@
       <c r="G140" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="H140" s="15"/>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="H140" s="16"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C141" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/spatial-transit.R</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H141" s="16"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B142" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C141" s="2" t="str">
+      <c r="C142" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-s3/scripts-ccao-data-warehouse-us-east-1/tax-bill_amount.R", "data-architecture/scripts-ccao-data-warehouse-us-east-1/tax-bill_amount.R")</f>
         <v>data-architecture/scripts-ccao-data-warehouse-us-east-1/tax-bill_amount.R</v>
       </c>
-      <c r="D141" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="E141" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G141" s="1" t="s">
+      <c r="E142" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G142" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H141" s="12" t="s">
+      <c r="H142" s="12" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
-      <c r="C142" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-access.sql", "data-architecture/aws-athena/ctas/location-access.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-access.sql</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G142" s="1"/>
-      <c r="H142" s="15" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-census.sql", "data-architecture/aws-athena/ctas/location-census.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-census.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-access.sql", "data-architecture/aws-athena/ctas/location-access.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-access.sql</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>12</v>
@@ -5298,17 +5321,19 @@
         <v>327</v>
       </c>
       <c r="G143" s="1"/>
-      <c r="H143" s="15"/>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="H143" s="16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-census_acs5.sql", "data-architecture/aws-athena/ctas/location-census_acs5.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-census_acs5.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-census.sql", "data-architecture/aws-athena/ctas/location-census.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-census.sql</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>12</v>
@@ -5317,17 +5342,17 @@
         <v>327</v>
       </c>
       <c r="G144" s="1"/>
-      <c r="H144" s="15"/>
-    </row>
-    <row r="145" spans="1:8">
+      <c r="H144" s="16"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-chicago.sql", "data-architecture/aws-athena/ctas/location-chicago.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-chicago.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-census_acs5.sql", "data-architecture/aws-athena/ctas/location-census_acs5.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-census_acs5.sql</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>12</v>
@@ -5336,17 +5361,17 @@
         <v>327</v>
       </c>
       <c r="G145" s="1"/>
-      <c r="H145" s="15"/>
-    </row>
-    <row r="146" spans="1:8">
+      <c r="H145" s="16"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-economy.sql", "data-architecture/aws-athena/ctas/location-economy.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-economy.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-chicago.sql", "data-architecture/aws-athena/ctas/location-chicago.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-chicago.sql</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>12</v>
@@ -5355,17 +5380,17 @@
         <v>327</v>
       </c>
       <c r="G146" s="1"/>
-      <c r="H146" s="15"/>
-    </row>
-    <row r="147" spans="1:8">
+      <c r="H146" s="16"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-environment.sql", "data-architecture/aws-athena/ctas/location-environment.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-environment.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-economy.sql", "data-architecture/aws-athena/ctas/location-economy.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-economy.sql</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>12</v>
@@ -5374,17 +5399,17 @@
         <v>327</v>
       </c>
       <c r="G147" s="1"/>
-      <c r="H147" s="15"/>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="H147" s="16"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-other.sql", "data-architecture/aws-athena/ctas/location-other.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-other.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-environment.sql", "data-architecture/aws-athena/ctas/location-environment.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-environment.sql</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>12</v>
@@ -5393,17 +5418,17 @@
         <v>327</v>
       </c>
       <c r="G148" s="1"/>
-      <c r="H148" s="15"/>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="H148" s="16"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-political.sql", "data-architecture/aws-athena/ctas/location-political.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-political.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-other.sql", "data-architecture/aws-athena/ctas/location-other.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-other.sql</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>12</v>
@@ -5412,17 +5437,17 @@
         <v>327</v>
       </c>
       <c r="G149" s="1"/>
-      <c r="H149" s="15"/>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="H149" s="16"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-school.sql", "data-architecture/aws-athena/ctas/location-school.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-school.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-political.sql", "data-architecture/aws-athena/ctas/location-political.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-political.sql</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>12</v>
@@ -5431,17 +5456,17 @@
         <v>327</v>
       </c>
       <c r="G150" s="1"/>
-      <c r="H150" s="15"/>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="H150" s="16"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-tax.sql", "data-architecture/aws-athena/ctas/location-tax.sql")</f>
-        <v>data-architecture/aws-athena/ctas/location-tax.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-school.sql", "data-architecture/aws-athena/ctas/location-school.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-school.sql</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>12</v>
@@ -5450,17 +5475,17 @@
         <v>327</v>
       </c>
       <c r="G151" s="1"/>
-      <c r="H151" s="15"/>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="H151" s="16"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-cnt_pin_num_bus_stop.sql", "data-architecture/aws-athena/ctas/proximity-cnt_pin_num_bus_stop.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-cnt_pin_num_bus_stop.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/location-tax.sql", "data-architecture/aws-athena/ctas/location-tax.sql")</f>
+        <v>data-architecture/aws-athena/ctas/location-tax.sql</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>12</v>
@@ -5469,19 +5494,17 @@
         <v>327</v>
       </c>
       <c r="G152" s="1"/>
-      <c r="H152" s="15" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="H152" s="16"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-cnt_pin_num_foreclosure.sql", "data-architecture/aws-athena/ctas/proximity-cnt_pin_num_foreclosure.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-cnt_pin_num_foreclosure.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-cnt_pin_num_bus_stop.sql", "data-architecture/aws-athena/ctas/proximity-cnt_pin_num_bus_stop.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-cnt_pin_num_bus_stop.sql</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>12</v>
@@ -5490,17 +5513,19 @@
         <v>327</v>
       </c>
       <c r="G153" s="1"/>
-      <c r="H153" s="15"/>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="H153" s="16" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-cnt_pin_num_school.sql", "data-architecture/aws-athena/ctas/proximity-cnt_pin_num_school.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-cnt_pin_num_school.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-cnt_pin_num_foreclosure.sql", "data-architecture/aws-athena/ctas/proximity-cnt_pin_num_foreclosure.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-cnt_pin_num_foreclosure.sql</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>12</v>
@@ -5509,17 +5534,17 @@
         <v>327</v>
       </c>
       <c r="G154" s="1"/>
-      <c r="H154" s="15"/>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="H154" s="16"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_bike_trail.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_bike_trail.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_bike_trail.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-cnt_pin_num_school.sql", "data-architecture/aws-athena/ctas/proximity-cnt_pin_num_school.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-cnt_pin_num_school.sql</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>12</v>
@@ -5528,17 +5553,17 @@
         <v>327</v>
       </c>
       <c r="G155" s="1"/>
-      <c r="H155" s="15"/>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="H155" s="16"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_cemetery.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_cemetery.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_cemetery.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_bike_trail.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_bike_trail.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_bike_trail.sql</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>12</v>
@@ -5547,17 +5572,17 @@
         <v>327</v>
       </c>
       <c r="G156" s="1"/>
-      <c r="H156" s="15"/>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="H156" s="16"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_cta_route.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_route.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_route.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_cemetery.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_cemetery.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_cemetery.sql</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>12</v>
@@ -5566,17 +5591,17 @@
         <v>327</v>
       </c>
       <c r="G157" s="1"/>
-      <c r="H157" s="15"/>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="H157" s="16"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_cta_stop.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_stop.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_stop.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_cta_route.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_route.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_route.sql</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>12</v>
@@ -5585,17 +5610,17 @@
         <v>327</v>
       </c>
       <c r="G158" s="1"/>
-      <c r="H158" s="15"/>
-    </row>
-    <row r="159" spans="1:8">
+      <c r="H158" s="16"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_hospital.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_hospital.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_hospital.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_cta_stop.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_stop.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_cta_stop.sql</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>12</v>
@@ -5604,17 +5629,17 @@
         <v>327</v>
       </c>
       <c r="G159" s="1"/>
-      <c r="H159" s="15"/>
-    </row>
-    <row r="160" spans="1:8">
+      <c r="H159" s="16"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_lake_michigan.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_lake_michigan.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_lake_michigan.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_hospital.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_hospital.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_hospital.sql</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>12</v>
@@ -5623,17 +5648,17 @@
         <v>327</v>
       </c>
       <c r="G160" s="1"/>
-      <c r="H160" s="15"/>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="H160" s="16"/>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_major_road.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_major_road.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_major_road.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_lake_michigan.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_lake_michigan.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_lake_michigan.sql</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>12</v>
@@ -5642,17 +5667,17 @@
         <v>327</v>
       </c>
       <c r="G161" s="1"/>
-      <c r="H161" s="15"/>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="H161" s="16"/>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_metra_route.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_route.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_route.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_major_road.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_major_road.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_major_road.sql</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>12</v>
@@ -5661,17 +5686,17 @@
         <v>327</v>
       </c>
       <c r="G162" s="1"/>
-      <c r="H162" s="15"/>
-    </row>
-    <row r="163" spans="1:8">
+      <c r="H162" s="16"/>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_metra_stop.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_stop.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_stop.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_metra_route.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_route.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_route.sql</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>12</v>
@@ -5680,17 +5705,17 @@
         <v>327</v>
       </c>
       <c r="G163" s="1"/>
-      <c r="H163" s="15"/>
-    </row>
-    <row r="164" spans="1:8">
+      <c r="H163" s="16"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_park.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_park.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_park.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_metra_stop.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_stop.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_metra_stop.sql</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>12</v>
@@ -5699,17 +5724,17 @@
         <v>327</v>
       </c>
       <c r="G164" s="1"/>
-      <c r="H164" s="15"/>
-    </row>
-    <row r="165" spans="1:8">
+      <c r="H164" s="16"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_pin.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_pin.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_pin.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_park.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_park.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_park.sql</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>12</v>
@@ -5718,17 +5743,17 @@
         <v>327</v>
       </c>
       <c r="G165" s="1"/>
-      <c r="H165" s="15"/>
-    </row>
-    <row r="166" spans="1:8">
+      <c r="H165" s="16"/>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_railroad.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_railroad.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_railroad.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_pin.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_pin.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_pin.sql</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>12</v>
@@ -5737,17 +5762,17 @@
         <v>327</v>
       </c>
       <c r="G166" s="1"/>
-      <c r="H166" s="15"/>
-    </row>
-    <row r="167" spans="1:8">
+      <c r="H166" s="16"/>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_water.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_water.sql")</f>
-        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_water.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_railroad.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_railroad.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_railroad.sql</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>12</v>
@@ -5756,17 +5781,17 @@
         <v>327</v>
       </c>
       <c r="G167" s="1"/>
-      <c r="H167" s="15"/>
-    </row>
-    <row r="168" spans="1:8">
+      <c r="H167" s="16"/>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/census-vw_acs5_stat.sql", "data-architecture/aws-athena/views/census-vw_acs5_stat.sql")</f>
-        <v>data-architecture/aws-athena/views/census-vw_acs5_stat.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/ctas/proximity-dist_pin_to_water.sql", "data-architecture/aws-athena/ctas/proximity-dist_pin_to_water.sql")</f>
+        <v>data-architecture/aws-athena/ctas/proximity-dist_pin_to_water.sql</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>12</v>
@@ -5775,40 +5800,38 @@
         <v>327</v>
       </c>
       <c r="G168" s="1"/>
-      <c r="H168" s="12" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8">
+      <c r="H168" s="16"/>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_card_res_char.sql", "data-architecture/aws-athena/views/default-vw_card_res_char.sql")</f>
-        <v>data-architecture/aws-athena/views/default-vw_card_res_char.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/census-vw_acs5_stat.sql", "data-architecture/aws-athena/views/census-vw_acs5_stat.sql")</f>
+        <v>data-architecture/aws-athena/views/census-vw_acs5_stat.sql</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>358</v>
+        <v>12</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="G169" s="1"/>
-      <c r="H169" s="15" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8">
+      <c r="H169" s="12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_condo_char.sql", "data-architecture/aws-athena/views/default-vw_pin_condo_char.sql")</f>
-        <v>data-architecture/aws-athena/views/default-vw_pin_condo_char.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_card_res_char.sql", "data-architecture/aws-athena/views/default-vw_card_res_char.sql")</f>
+        <v>data-architecture/aws-athena/views/default-vw_card_res_char.sql</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>358</v>
@@ -5817,17 +5840,19 @@
         <v>359</v>
       </c>
       <c r="G170" s="1"/>
-      <c r="H170" s="15"/>
-    </row>
-    <row r="171" spans="1:8">
+      <c r="H170" s="16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_history.sql", "data-architecture/aws-athena/views/default-vw_pin_history.sql")</f>
-        <v>data-architecture/aws-athena/views/default-vw_pin_history.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_condo_char.sql", "data-architecture/aws-athena/views/default-vw_pin_condo_char.sql")</f>
+        <v>data-architecture/aws-athena/views/default-vw_pin_condo_char.sql</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>358</v>
@@ -5836,19 +5861,17 @@
         <v>359</v>
       </c>
       <c r="G171" s="1"/>
-      <c r="H171" s="12" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="H171" s="16"/>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_sale.sql", "data-architecture/aws-athena/views/default-vw_pin_sale.sql")</f>
-        <v>data-architecture/aws-athena/views/default-vw_pin_sale.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_history.sql", "data-architecture/aws-athena/views/default-vw_pin_history.sql")</f>
+        <v>data-architecture/aws-athena/views/default-vw_pin_history.sql</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>358</v>
@@ -5858,18 +5881,18 @@
       </c>
       <c r="G172" s="1"/>
       <c r="H172" s="12" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_universe.sql", "data-architecture/aws-athena/views/default-vw_pin_universe.sql")</f>
-        <v>data-architecture/aws-athena/views/default-vw_pin_universe.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_sale.sql", "data-architecture/aws-athena/views/default-vw_pin_sale.sql")</f>
+        <v>data-architecture/aws-athena/views/default-vw_pin_sale.sql</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>358</v>
@@ -5879,18 +5902,18 @@
       </c>
       <c r="G173" s="1"/>
       <c r="H173" s="12" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/location-vw_pin10_location.sql", "data-architecture/aws-athena/views/location-vw_pin10_location.sql")</f>
-        <v>data-architecture/aws-athena/views/location-vw_pin10_location.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/default-vw_pin_universe.sql", "data-architecture/aws-athena/views/default-vw_pin_universe.sql")</f>
+        <v>data-architecture/aws-athena/views/default-vw_pin_universe.sql</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>358</v>
@@ -5900,18 +5923,18 @@
       </c>
       <c r="G174" s="1"/>
       <c r="H174" s="12" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/model-vw_card_res_input.sql", "data-architecture/aws-athena/views/model-vw_card_res_input.sql")</f>
-        <v>data-architecture/aws-athena/views/model-vw_card_res_input.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/location-vw_pin10_location.sql", "data-architecture/aws-athena/views/location-vw_pin10_location.sql")</f>
+        <v>data-architecture/aws-athena/views/location-vw_pin10_location.sql</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>358</v>
@@ -5920,19 +5943,19 @@
         <v>359</v>
       </c>
       <c r="G175" s="1"/>
-      <c r="H175" s="15" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8">
+      <c r="H175" s="12" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/model-vw_pin_condo_input.sql", "data-architecture/aws-athena/views/model-vw_pin_condo_input.sql")</f>
-        <v>data-architecture/aws-athena/views/model-vw_pin_condo_input.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/model-vw_card_res_input.sql", "data-architecture/aws-athena/views/model-vw_card_res_input.sql")</f>
+        <v>data-architecture/aws-athena/views/model-vw_card_res_input.sql</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>358</v>
@@ -5941,17 +5964,19 @@
         <v>359</v>
       </c>
       <c r="G176" s="1"/>
-      <c r="H176" s="15"/>
-    </row>
-    <row r="177" spans="1:8">
+      <c r="H176" s="16" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/model-vw_card_shap_long.sql", "data-architecture/aws-athena/views/model-vw_card_shap_long.sql")</f>
-        <v>data-architecture/aws-athena/views/model-vw_card_shap_long.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/model-vw_pin_condo_input.sql", "data-architecture/aws-athena/views/model-vw_pin_condo_input.sql")</f>
+        <v>data-architecture/aws-athena/views/model-vw_pin_condo_input.sql</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>358</v>
@@ -5960,19 +5985,17 @@
         <v>359</v>
       </c>
       <c r="G177" s="1"/>
-      <c r="H177" s="12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8">
+      <c r="H177" s="16"/>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/proximity-vw_pin10_proximity.sql", "data-architecture/aws-athena/views/proximity-vw_pin10_proximity.sql")</f>
-        <v>data-architecture/aws-athena/views/proximity-vw_pin10_proximity.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/model-vw_card_shap_long.sql", "data-architecture/aws-athena/views/model-vw_card_shap_long.sql")</f>
+        <v>data-architecture/aws-athena/views/model-vw_card_shap_long.sql</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>358</v>
@@ -5982,18 +6005,18 @@
       </c>
       <c r="G178" s="1"/>
       <c r="H178" s="12" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="2" t="str">
-        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/rpie-vw_pin_class_flatfile.sql", "data-architecture/aws-athena/views/rpie-vw_pin_class_flatfile.sql")</f>
-        <v>data-architecture/aws-athena/views/rpie-vw_pin_class_flatfile.sql</v>
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/proximity-vw_pin10_proximity.sql", "data-architecture/aws-athena/views/proximity-vw_pin10_proximity.sql")</f>
+        <v>data-architecture/aws-athena/views/proximity-vw_pin10_proximity.sql</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>358</v>
@@ -6003,51 +6026,73 @@
       </c>
       <c r="G179" s="1"/>
       <c r="H179" s="12" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="2" t="str">
+        <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/rpie-vw_pin_class_flatfile.sql", "data-architecture/aws-athena/views/rpie-vw_pin_class_flatfile.sql")</f>
+        <v>data-architecture/aws-athena/views/rpie-vw_pin_class_flatfile.sql</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G180" s="1"/>
+      <c r="H180" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="2" t="str">
         <f>HYPERLINK("https://gitlab.com/ccao-data-science---modeling/data-architecture/-/blob/master/aws-athena/views/rpie-vw_pin_mailers.sql", "data-architecture/aws-athena/views/rpie-vw_pin_mailers.sql")</f>
         <v>data-architecture/aws-athena/views/rpie-vw_pin_mailers.sql</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D181" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="E180" s="1" t="s">
+      <c r="E181" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="F180" s="1" t="s">
+      <c r="F181" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="G180" s="1"/>
-      <c r="H180" s="12" t="s">
+      <c r="G181" s="1"/>
+      <c r="H181" s="12" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I180" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I181" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="17">
-    <mergeCell ref="H152:H167"/>
-    <mergeCell ref="H169:H170"/>
-    <mergeCell ref="H175:H176"/>
-    <mergeCell ref="H79:H81"/>
-    <mergeCell ref="H123:H125"/>
-    <mergeCell ref="H127:H133"/>
-    <mergeCell ref="H83:H84"/>
-    <mergeCell ref="H101:H102"/>
-    <mergeCell ref="H142:H151"/>
     <mergeCell ref="H8:H24"/>
     <mergeCell ref="H25:H27"/>
     <mergeCell ref="H85:H98"/>
     <mergeCell ref="H37:H67"/>
-    <mergeCell ref="H138:H140"/>
-    <mergeCell ref="H135:H137"/>
+    <mergeCell ref="H139:H141"/>
+    <mergeCell ref="H136:H138"/>
     <mergeCell ref="H28:H31"/>
     <mergeCell ref="H34:H35"/>
+    <mergeCell ref="H153:H168"/>
+    <mergeCell ref="H170:H171"/>
+    <mergeCell ref="H176:H177"/>
+    <mergeCell ref="H79:H81"/>
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="H128:H134"/>
+    <mergeCell ref="H83:H84"/>
+    <mergeCell ref="H101:H102"/>
+    <mergeCell ref="H143:H152"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6063,12 +6108,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B10A1146621544CA10AFFB6B345C290" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7de3d23f6a217b71996bb76c6e8b64d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c" xmlns:ns3="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7e828ff3871c9f261bef45e53781f93" ns2:_="" ns3:_="">
     <xsd:import namespace="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
@@ -6259,14 +6298,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5AE86BA-1E3B-4FEE-879B-15C0E7DA7515}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5AE86BA-1E3B-4FEE-879B-15C0E7DA7515}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF32FFB-975E-4BAA-AC25-B80C1A2F0602}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6333D1F-7E57-44A3-BAB8-D3D3045717FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="20f740d3-e7cb-4f0f-9e63-8fcc8a32785c"/>
+    <ds:schemaRef ds:uri="b7d6f9e3-881f-4519-a9f9-0856d2ed65b9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6333D1F-7E57-44A3-BAB8-D3D3045717FD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF32FFB-975E-4BAA-AC25-B80C1A2F0602}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>